<commit_message>
new begenning. Basic biomass, coexistence and cover analisys/plot. Also some data organisations.
</commit_message>
<xml_diff>
--- a/oster_data_2022/enz_act.xlsx
+++ b/oster_data_2022/enz_act.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathis\Documents\Fac\Cesure2\Plant species coexistence\functions_and_coex\oster_data_2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathis\Documents\Fac\Cesure2\Plant_species_coexistence\functions_and_coex\oster_data_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A235395-D804-48C3-BF31-54E79D622D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0385573A-94CA-4743-9577-1DCD9090AC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="14">
   <si>
     <t>Abs</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>cali_group</t>
+  </si>
+  <si>
+    <t>cali</t>
   </si>
 </sst>
 </file>
@@ -430,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A141" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
+      <selection activeCell="C447" sqref="C447:C455"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -471,7 +474,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>5</v>
@@ -494,7 +497,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>5</v>
@@ -517,7 +520,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>5</v>
@@ -540,7 +543,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>5</v>
@@ -563,7 +566,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>5</v>
@@ -586,7 +589,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>5</v>
@@ -609,7 +612,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>5</v>
@@ -632,7 +635,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>5</v>
@@ -655,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>5</v>
@@ -4418,7 +4421,7 @@
         <v>2</v>
       </c>
       <c r="C189" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D189" s="5" t="s">
         <v>5</v>
@@ -4441,7 +4444,7 @@
         <v>2</v>
       </c>
       <c r="C190" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D190" s="5" t="s">
         <v>5</v>
@@ -4464,7 +4467,7 @@
         <v>2</v>
       </c>
       <c r="C191" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D191" s="5" t="s">
         <v>5</v>
@@ -4487,7 +4490,7 @@
         <v>2</v>
       </c>
       <c r="C192" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D192" s="5" t="s">
         <v>5</v>
@@ -4510,7 +4513,7 @@
         <v>2</v>
       </c>
       <c r="C193" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D193" s="5" t="s">
         <v>5</v>
@@ -4533,7 +4536,7 @@
         <v>2</v>
       </c>
       <c r="C194" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D194" s="5" t="s">
         <v>5</v>
@@ -4556,7 +4559,7 @@
         <v>2</v>
       </c>
       <c r="C195" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D195" s="5" t="s">
         <v>5</v>
@@ -4579,7 +4582,7 @@
         <v>2</v>
       </c>
       <c r="C196" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D196" s="5" t="s">
         <v>5</v>
@@ -4602,7 +4605,7 @@
         <v>2</v>
       </c>
       <c r="C197" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D197" s="5" t="s">
         <v>5</v>
@@ -6302,7 +6305,7 @@
         <v>9</v>
       </c>
       <c r="C278" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D278" s="5" t="s">
         <v>5</v>
@@ -6325,7 +6328,7 @@
         <v>9</v>
       </c>
       <c r="C279" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D279" s="5" t="s">
         <v>5</v>
@@ -6348,7 +6351,7 @@
         <v>9</v>
       </c>
       <c r="C280" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D280" s="5" t="s">
         <v>5</v>
@@ -6371,7 +6374,7 @@
         <v>9</v>
       </c>
       <c r="C281" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D281" s="5" t="s">
         <v>5</v>
@@ -6394,7 +6397,7 @@
         <v>9</v>
       </c>
       <c r="C282" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D282" s="5" t="s">
         <v>5</v>
@@ -6417,7 +6420,7 @@
         <v>9</v>
       </c>
       <c r="C283" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D283" s="5" t="s">
         <v>5</v>
@@ -6440,7 +6443,7 @@
         <v>9</v>
       </c>
       <c r="C284" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D284" s="5" t="s">
         <v>5</v>
@@ -6463,7 +6466,7 @@
         <v>9</v>
       </c>
       <c r="C285" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D285" s="5" t="s">
         <v>5</v>
@@ -6486,7 +6489,7 @@
         <v>9</v>
       </c>
       <c r="C286" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D286" s="5" t="s">
         <v>5</v>
@@ -9944,7 +9947,7 @@
         <v>9</v>
       </c>
       <c r="C447" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D447" s="5" t="s">
         <v>5</v>
@@ -9967,7 +9970,7 @@
         <v>9</v>
       </c>
       <c r="C448" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D448" s="5" t="s">
         <v>5</v>
@@ -9990,7 +9993,7 @@
         <v>9</v>
       </c>
       <c r="C449" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D449" s="5" t="s">
         <v>5</v>
@@ -10013,7 +10016,7 @@
         <v>9</v>
       </c>
       <c r="C450" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D450" s="5" t="s">
         <v>5</v>
@@ -10036,7 +10039,7 @@
         <v>9</v>
       </c>
       <c r="C451" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D451" s="5" t="s">
         <v>5</v>
@@ -10059,7 +10062,7 @@
         <v>9</v>
       </c>
       <c r="C452" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D452" s="5" t="s">
         <v>5</v>
@@ -10082,7 +10085,7 @@
         <v>9</v>
       </c>
       <c r="C453" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D453" s="5" t="s">
         <v>5</v>
@@ -10105,7 +10108,7 @@
         <v>9</v>
       </c>
       <c r="C454" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D454" s="5" t="s">
         <v>5</v>
@@ -10128,7 +10131,7 @@
         <v>9</v>
       </c>
       <c r="C455" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D455" s="5" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
data in txt files almost done, some codes and files cleaning left
</commit_message>
<xml_diff>
--- a/oster_data_2022/enz_act.xlsx
+++ b/oster_data_2022/enz_act.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mathis\Documents\Fac\Cesure2\Plant_species_coexistence\functions_and_coex\oster_data_2022\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0385573A-94CA-4743-9577-1DCD9090AC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F7448F6-4105-45E2-93E1-FDDF77B8BA79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -433,8 +433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G542"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A436" workbookViewId="0">
-      <selection activeCell="C447" sqref="C447:C455"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="D99" sqref="D99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1081,7 +1081,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>5</v>
@@ -1104,7 +1104,7 @@
         <v>2</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>5</v>
@@ -1127,7 +1127,7 @@
         <v>2</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>5</v>
@@ -1150,7 +1150,7 @@
         <v>2</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>5</v>
@@ -1173,7 +1173,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D35" s="5" t="s">
         <v>5</v>
@@ -1196,7 +1196,7 @@
         <v>2</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D36" s="5" t="s">
         <v>5</v>
@@ -1219,7 +1219,7 @@
         <v>2</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>5</v>
@@ -1242,7 +1242,7 @@
         <v>2</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>5</v>
@@ -1265,7 +1265,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D39" s="5" t="s">
         <v>5</v>
@@ -2460,7 +2460,7 @@
         <v>2</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>5</v>
@@ -2483,7 +2483,7 @@
         <v>2</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>5</v>
@@ -2506,7 +2506,7 @@
         <v>2</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>5</v>
@@ -2529,7 +2529,7 @@
         <v>2</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>5</v>
@@ -2552,7 +2552,7 @@
         <v>2</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>5</v>
@@ -2575,7 +2575,7 @@
         <v>2</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>5</v>
@@ -2598,7 +2598,7 @@
         <v>2</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>5</v>
@@ -2621,7 +2621,7 @@
         <v>2</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>5</v>
@@ -2644,7 +2644,7 @@
         <v>2</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>5</v>

</xml_diff>